<commit_message>
fix statistics and plot issue
</commit_message>
<xml_diff>
--- a/excel/market_analysis.xlsx
+++ b/excel/market_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trading\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CE9E67-B667-4C2A-8012-23250A0E3AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489F8F84-8126-489B-8F49-B885A7527848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DX230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ190" workbookViewId="0">
-      <selection activeCell="DS200" sqref="DS200"/>
+    <sheetView tabSelected="1" topLeftCell="CZ196" workbookViewId="0">
+      <selection activeCell="DX232" sqref="DX232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -64424,8 +64424,14 @@
       <c r="CU209">
         <v>2.94</v>
       </c>
+      <c r="DM209">
+        <v>4.37</v>
+      </c>
+      <c r="DN209">
+        <v>2.5099999999999998</v>
+      </c>
       <c r="DO209">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="DP209">
         <v>3.7</v>
@@ -65838,8 +65844,14 @@
       <c r="CU214">
         <v>27.27</v>
       </c>
+      <c r="DM214">
+        <v>2.64</v>
+      </c>
+      <c r="DN214">
+        <v>2.76</v>
+      </c>
       <c r="DO214">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="DP214">
         <v>3.35</v>
@@ -66400,8 +66412,14 @@
       <c r="CU216">
         <v>4.3499999999999996</v>
       </c>
+      <c r="DM216">
+        <v>2.13</v>
+      </c>
+      <c r="DN216">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="DO216">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="DP216">
         <v>1.9</v>
@@ -68280,8 +68298,14 @@
       <c r="CU223">
         <v>17.649999999999999</v>
       </c>
+      <c r="DM223">
+        <v>2.46</v>
+      </c>
+      <c r="DN223">
+        <v>4.67</v>
+      </c>
       <c r="DO223">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="DP223">
         <v>3.9</v>
@@ -68860,11 +68884,14 @@
       <c r="DR225">
         <v>3</v>
       </c>
+      <c r="DS225">
+        <v>-2.2200000000000002</v>
+      </c>
       <c r="DT225">
         <v>-5.25</v>
       </c>
       <c r="DU225">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="DV225">
         <v>0.39</v>
@@ -69691,8 +69718,14 @@
       <c r="CU228">
         <v>34.78</v>
       </c>
+      <c r="DM228">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="DN228">
+        <v>0.97</v>
+      </c>
       <c r="DO228">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="DP228">
         <v>3.53</v>

</xml_diff>

<commit_message>
update datas and change param
</commit_message>
<xml_diff>
--- a/excel/market_analysis.xlsx
+++ b/excel/market_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DM288"/>
+  <dimension ref="A1:DM289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -90179,6 +90179,295 @@
         </is>
       </c>
     </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>20260106</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>4108</v>
+      </c>
+      <c r="C289" t="n">
+        <v>1222</v>
+      </c>
+      <c r="D289" t="n">
+        <v>129</v>
+      </c>
+      <c r="E289" t="n">
+        <v>395</v>
+      </c>
+      <c r="F289" t="n">
+        <v>28</v>
+      </c>
+      <c r="G289" t="n">
+        <v>224</v>
+      </c>
+      <c r="H289" t="n">
+        <v>8</v>
+      </c>
+      <c r="I289" t="n">
+        <v>162</v>
+      </c>
+      <c r="J289" t="n">
+        <v>3</v>
+      </c>
+      <c r="K289" t="n">
+        <v>120</v>
+      </c>
+      <c r="L289" t="n">
+        <v>1</v>
+      </c>
+      <c r="M289" t="n">
+        <v>47</v>
+      </c>
+      <c r="N289" t="n">
+        <v>25</v>
+      </c>
+      <c r="O289" t="n">
+        <v>108</v>
+      </c>
+      <c r="P289" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="Q289" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="R289" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="S289" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="T289" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="U289" t="n">
+        <v>13.06</v>
+      </c>
+      <c r="V289" t="n">
+        <v>14.92</v>
+      </c>
+      <c r="W289" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="X289" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="Y289" t="n">
+        <v>80.56</v>
+      </c>
+      <c r="Z289" t="n">
+        <v>82.41</v>
+      </c>
+      <c r="AA289" t="n">
+        <v>59.26</v>
+      </c>
+      <c r="AB289" t="n">
+        <v>100</v>
+      </c>
+      <c r="AC289" t="n">
+        <v>97.22</v>
+      </c>
+      <c r="AD289" t="n">
+        <v>80.56</v>
+      </c>
+      <c r="AE289" t="n">
+        <v>82.41</v>
+      </c>
+      <c r="AF289" t="n">
+        <v>18</v>
+      </c>
+      <c r="AG289" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="AH289" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="AI289" t="n">
+        <v>7.54</v>
+      </c>
+      <c r="AJ289" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="AK289" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="AL289" t="n">
+        <v>7.87</v>
+      </c>
+      <c r="AM289" t="n">
+        <v>10.83</v>
+      </c>
+      <c r="AN289" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="AO289" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="AP289" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="AQ289" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="AR289" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="AS289" t="n">
+        <v>100</v>
+      </c>
+      <c r="AT289" t="n">
+        <v>88.89</v>
+      </c>
+      <c r="AU289" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="AV289" t="n">
+        <v>72.22</v>
+      </c>
+      <c r="AW289" t="inlineStr"/>
+      <c r="AX289" t="inlineStr"/>
+      <c r="AY289" t="inlineStr"/>
+      <c r="AZ289" t="inlineStr"/>
+      <c r="BA289" t="inlineStr"/>
+      <c r="BB289" t="inlineStr"/>
+      <c r="BC289" t="inlineStr"/>
+      <c r="BD289" t="inlineStr"/>
+      <c r="BE289" t="inlineStr"/>
+      <c r="BF289" t="inlineStr"/>
+      <c r="BG289" t="inlineStr"/>
+      <c r="BH289" t="inlineStr"/>
+      <c r="BI289" t="inlineStr"/>
+      <c r="BJ289" t="inlineStr"/>
+      <c r="BK289" t="inlineStr"/>
+      <c r="BL289" t="inlineStr"/>
+      <c r="BM289" t="inlineStr"/>
+      <c r="BN289" t="n">
+        <v>8</v>
+      </c>
+      <c r="BO289" t="n">
+        <v>-3.98</v>
+      </c>
+      <c r="BP289" t="n">
+        <v>-1.34</v>
+      </c>
+      <c r="BQ289" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="BR289" t="n">
+        <v>-5.67</v>
+      </c>
+      <c r="BS289" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="BT289" t="n">
+        <v>-9.6</v>
+      </c>
+      <c r="BU289" t="n">
+        <v>-7.25</v>
+      </c>
+      <c r="BV289" t="n">
+        <v>-11.14</v>
+      </c>
+      <c r="BW289" t="n">
+        <v>-8.85</v>
+      </c>
+      <c r="BX289" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY289" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="BZ289" t="n">
+        <v>62.5</v>
+      </c>
+      <c r="CA289" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB289" t="n">
+        <v>0</v>
+      </c>
+      <c r="CC289" t="n">
+        <v>0</v>
+      </c>
+      <c r="CD289" t="n">
+        <v>0</v>
+      </c>
+      <c r="CE289" t="n">
+        <v>26</v>
+      </c>
+      <c r="CF289" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="CG289" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="CH289" t="n">
+        <v>3.91</v>
+      </c>
+      <c r="CI289" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="CJ289" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="CK289" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="CL289" t="n">
+        <v>4.41</v>
+      </c>
+      <c r="CM289" t="n">
+        <v>-3.99</v>
+      </c>
+      <c r="CN289" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="CO289" t="n">
+        <v>34.62</v>
+      </c>
+      <c r="CP289" t="n">
+        <v>57.69</v>
+      </c>
+      <c r="CQ289" t="n">
+        <v>65.38</v>
+      </c>
+      <c r="CR289" t="n">
+        <v>73.08</v>
+      </c>
+      <c r="CS289" t="n">
+        <v>80.77</v>
+      </c>
+      <c r="CT289" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="CU289" t="n">
+        <v>23.08</v>
+      </c>
+      <c r="CV289" t="inlineStr"/>
+      <c r="CW289" t="inlineStr"/>
+      <c r="CX289" t="inlineStr"/>
+      <c r="CY289" t="inlineStr"/>
+      <c r="CZ289" t="inlineStr"/>
+      <c r="DA289" t="inlineStr"/>
+      <c r="DB289" t="inlineStr"/>
+      <c r="DC289" t="inlineStr"/>
+      <c r="DD289" t="inlineStr"/>
+      <c r="DE289" t="inlineStr"/>
+      <c r="DF289" t="inlineStr"/>
+      <c r="DG289" t="inlineStr"/>
+      <c r="DH289" t="inlineStr"/>
+      <c r="DI289" t="inlineStr"/>
+      <c r="DJ289" t="inlineStr"/>
+      <c r="DK289" t="inlineStr"/>
+      <c r="DL289" t="inlineStr"/>
+      <c r="DM289" t="inlineStr">
+        <is>
+          <t>{"0": {"开盘": 5.27, "收盘": 6.48, "样本": 55}, "1": {"开盘": 3.43, "收盘": 6.07, "样本": 22}, "2": {"开盘": 3.18, "收盘": 2.9, "样本": 5}, "3": {"开盘": 4.32, "收盘": 5.8, "样本": 14}, "4": {"开盘": 4.25, "收盘": 8.86, "样本": 6}, "5": {"开盘": 0.0, "收盘": 7.11, "样本": 1}, "6": {"开盘": -0.22, "收盘": 2.48, "样本": 1}, "7": {"开盘": 5.36, "收盘": 9.99, "样本": 1}, "8": {"开盘": 0.0, "收盘": -3.64, "样本": 1}, "10": {"开盘": 13.99, "收盘": 20.0, "样本": 1}, "12": {"开盘": 2.28, "收盘": 0.55, "样本": 1}}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>